<commit_message>
Mostly finished profile management
Cant get reentering the password to work
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -404,7 +404,15 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Actual</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -528,10 +536,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$27</c:f>
+              <c:f>Sheet1!$C$3:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>41</c:v>
                 </c:pt>
@@ -603,6 +611,12 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -619,11 +633,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-27145024"/>
-        <c:axId val="-27156992"/>
+        <c:axId val="505552720"/>
+        <c:axId val="505542928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-27145024"/>
+        <c:axId val="505552720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -722,7 +736,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-27156992"/>
+        <c:crossAx val="505542928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -730,7 +744,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-27156992"/>
+        <c:axId val="505542928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,7 +851,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-27145024"/>
+        <c:crossAx val="505552720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1729,8 +1743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2062,6 +2076,9 @@
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
+      <c r="C27">
+        <v>25</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -2070,6 +2087,9 @@
       <c r="B28">
         <f t="shared" si="0"/>
         <v>4</v>
+      </c>
+      <c r="C28">
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated for todays work
Miscalculated how much tasks we really had in the beginning but, the
graph still shows the same general pattern
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -309,88 +309,88 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>41</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.5</c:v>
+                  <c:v>36.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37</c:v>
+                  <c:v>35.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.5</c:v>
+                  <c:v>33.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34</c:v>
+                  <c:v>32.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.5</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31</c:v>
+                  <c:v>29.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.5</c:v>
+                  <c:v>28.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>28</c:v>
+                  <c:v>26.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>26.5</c:v>
+                  <c:v>25.4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23.5</c:v>
+                  <c:v>22.6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>22</c:v>
+                  <c:v>21.2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.5</c:v>
+                  <c:v>19.8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>19</c:v>
+                  <c:v>18.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17.5</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16</c:v>
+                  <c:v>15.6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14.5</c:v>
+                  <c:v>14.2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13</c:v>
+                  <c:v>12.8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.5</c:v>
+                  <c:v>11.4</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.5</c:v>
+                  <c:v>8.6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7</c:v>
+                  <c:v>7.2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.5</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
@@ -541,22 +541,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>41</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>33</c:v>
@@ -568,55 +568,58 @@
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>19</c:v>
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -633,11 +636,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="505552720"/>
-        <c:axId val="505542928"/>
+        <c:axId val="-56323328"/>
+        <c:axId val="-56322784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="505552720"/>
+        <c:axId val="-56323328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +739,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="505542928"/>
+        <c:crossAx val="-56322784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -744,7 +747,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="505542928"/>
+        <c:axId val="-56322784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -851,7 +854,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="505552720"/>
+        <c:crossAx val="-56323328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1743,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,10 +1777,10 @@
         <v>28</v>
       </c>
       <c r="B3">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -1792,10 +1795,10 @@
       </c>
       <c r="B4">
         <f xml:space="preserve"> ROUND(B3 - (B$3 / 28),0)</f>
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E4" s="1">
         <v>42604</v>
@@ -1810,10 +1813,10 @@
       </c>
       <c r="B5">
         <f t="shared" ref="B5:B29" si="0" xml:space="preserve"> ROUND(B4 - (B$3 / 28),1)</f>
-        <v>38.5</v>
+        <v>36.6</v>
       </c>
       <c r="C5">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1822,10 +1825,10 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="C6">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1834,10 +1837,10 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>35.5</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="C7">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1846,10 +1849,10 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>32.4</v>
       </c>
       <c r="C8">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1858,7 +1861,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>32.5</v>
+        <v>31</v>
       </c>
       <c r="C9">
         <v>33</v>
@@ -1870,7 +1873,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>29.6</v>
       </c>
       <c r="C10">
         <v>33</v>
@@ -1882,7 +1885,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>29.5</v>
+        <v>28.2</v>
       </c>
       <c r="C11">
         <v>33</v>
@@ -1894,10 +1897,10 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>26.8</v>
       </c>
       <c r="C12">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1906,10 +1909,10 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>26.5</v>
+        <v>25.4</v>
       </c>
       <c r="C13">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1918,10 +1921,10 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1930,10 +1933,10 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>23.5</v>
+        <v>22.6</v>
       </c>
       <c r="C15">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1942,10 +1945,10 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
+        <v>21.2</v>
+      </c>
+      <c r="C16">
         <v>22</v>
-      </c>
-      <c r="C16">
-        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1954,10 +1957,10 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>20.5</v>
+        <v>19.8</v>
       </c>
       <c r="C17">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1966,10 +1969,10 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="C18">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1978,10 +1981,10 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>17.5</v>
+        <v>17</v>
       </c>
       <c r="C19">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1990,10 +1993,10 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15.6</v>
       </c>
       <c r="C20">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2002,10 +2005,10 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>14.2</v>
       </c>
       <c r="C21">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2014,10 +2017,10 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12.8</v>
       </c>
       <c r="C22">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2026,10 +2029,10 @@
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>11.5</v>
+        <v>11.4</v>
       </c>
       <c r="C23">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2041,7 +2044,7 @@
         <v>10</v>
       </c>
       <c r="C24">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2050,10 +2053,10 @@
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="C25">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2062,10 +2065,10 @@
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>7.2</v>
       </c>
       <c r="C26">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2074,10 +2077,10 @@
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>5.5</v>
+        <v>5.8</v>
       </c>
       <c r="C27">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2086,10 +2089,10 @@
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C28">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2098,7 +2101,10 @@
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2107,7 +2113,7 @@
       </c>
       <c r="B30">
         <f xml:space="preserve"> ROUND(B29 - (B$3 / 28),1)</f>
-        <v>1</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2115,7 +2121,7 @@
         <v>0</v>
       </c>
       <c r="B31">
-        <f xml:space="preserve"> MAX(0,ROUND(B30 - (B$3 / 28),1))</f>
+        <f>ROUND(B30-(B$3/28),0)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalised with release one work
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\QUT\Year 2\Sem 2\IFB299\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\QUT\Year 2\Sem 2\IFB299\IFB299-Group23\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -624,6 +624,9 @@
                 <c:pt idx="27">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -639,11 +642,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1627009808"/>
-        <c:axId val="-1627003280"/>
+        <c:axId val="312917024"/>
+        <c:axId val="312917568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1627009808"/>
+        <c:axId val="312917024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -742,7 +745,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1627003280"/>
+        <c:crossAx val="312917568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -750,7 +753,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1627003280"/>
+        <c:axId val="312917568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -857,7 +860,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1627009808"/>
+        <c:crossAx val="312917024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1749,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,6 +2133,9 @@
         <f>ROUND(B30-(B$3/28),0)</f>
         <v>0</v>
       </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
The support docs for sprint 3
Dont get intimidated by the large amount of tasks. Most of it comes
styling.

Essentially what i was thinking was making the already existing website
as a homepage for none members. Then as registered users (member,
planner, volunteer) uses these webpages after the login.

This time around were gonna build each page one by one. I know it might
be slow, but its easier to divide the work up this way. Most of the
tasks and user stories should be modulor, as in you can build the page
for a tab, then over time just add the links to allow it to connect to
other pages. Also you have to apply styling which havent done, so for
now just focus on creating functionality, displaying the required info,
forms with textboxes, sql queries are working etc.

If you want a storyboardish/overview dataflow type diagram go to my
personal portfolio or google drive under release 2, to find the designs.
Thats where i based these tasks on, most user stories are one tab.
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -2,17 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\QUT\Year 2\Sem 2\IFB299\IFB299-Group23\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\QUT\Year 2\Sem 2\IFB299\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Days</t>
   </si>
@@ -140,7 +141,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -624,9 +624,6 @@
                 <c:pt idx="27">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="28">
-                  <c:v>2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -642,11 +639,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="312917024"/>
-        <c:axId val="312917568"/>
+        <c:axId val="-1945614640"/>
+        <c:axId val="-1945608656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="312917024"/>
+        <c:axId val="-1945614640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -675,6 +672,677 @@
                   <a:rPr lang="en-AU"/>
                   <a:t>Days Till Release 1</a:t>
                 </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1945608656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1945608656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Tasks to be done</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1945614640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Sprint 3 Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sprint3!$A$3:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint3!$B$3:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85.71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.42</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77.13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72.84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>68.55</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.260000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59.97</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55.68</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51.39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>47.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42.81</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>38.520000000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>34.229999999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29.94</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25.65</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21.36</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.07</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12.78</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.49</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sprint3!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sprint3!$A$3:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint3!$C$3:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-1945611376"/>
+        <c:axId val="-1945613008"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1945611376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Days Till release</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> one</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -745,7 +1413,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312917568"/>
+        <c:crossAx val="-1945613008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -753,7 +1421,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="312917568"/>
+        <c:axId val="-1945613008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -860,7 +1528,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312917024"/>
+        <c:crossAx val="-1945611376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -949,7 +1617,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1471,6 +2682,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1750,9 +2998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -2133,8 +3382,263 @@
         <f>ROUND(B30-(B$3/28),0)</f>
         <v>0</v>
       </c>
-      <c r="C31">
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>90</v>
+      </c>
+      <c r="C3">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <f xml:space="preserve"> ROUND(B3 - (B$3 / 21),2)</f>
+        <v>85.71</v>
+      </c>
+      <c r="C4">
+        <v>90</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42632</v>
+      </c>
+      <c r="F4" s="1">
+        <v>42653</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B23" si="0" xml:space="preserve"> ROUND(B4 - (B$3 / 21),2)</f>
+        <v>81.42</v>
+      </c>
+      <c r="C5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>77.13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>72.84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>68.55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>64.260000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>59.97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>55.68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>51.39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>47.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>42.81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>38.520000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>34.229999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>29.94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>25.65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>21.36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>17.07</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>12.78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>8.49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <f xml:space="preserve"> ROUND(B23 - (B$3 / 21),0)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Just noticed there wasnt a table for some tasks
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -639,11 +639,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1945614640"/>
-        <c:axId val="-1945608656"/>
+        <c:axId val="-710436544"/>
+        <c:axId val="-710439808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1945614640"/>
+        <c:axId val="-710436544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -741,7 +741,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1945608656"/>
+        <c:crossAx val="-710439808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -749,7 +749,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1945608656"/>
+        <c:axId val="-710439808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1945614640"/>
+        <c:crossAx val="-710436544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1288,7 +1288,7 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1305,11 +1305,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1945611376"/>
-        <c:axId val="-1945613008"/>
+        <c:axId val="-710435456"/>
+        <c:axId val="-710432192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1945611376"/>
+        <c:axId val="-710435456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1413,7 +1413,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1945613008"/>
+        <c:crossAx val="-710432192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1421,7 +1421,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1945613008"/>
+        <c:axId val="-710432192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1528,7 +1528,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1945611376"/>
+        <c:crossAx val="-710435456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3398,7 +3398,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3467,7 +3467,7 @@
         <v>81.42</v>
       </c>
       <c r="C5">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FInished the login feature, still gotta do account page
Also theres a template there. You can just copy that and edit for
whatever tab your working on. It should carry the CSS stylings
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\QUT\Year 2\Sem 2\IFB299\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\QUT\Year 2\Sem 2\IFB299\IFB299-Group23\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -639,11 +639,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-710436544"/>
-        <c:axId val="-710439808"/>
+        <c:axId val="2077942944"/>
+        <c:axId val="2077944576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-710436544"/>
+        <c:axId val="2077942944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -741,7 +741,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-710439808"/>
+        <c:crossAx val="2077944576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -749,7 +749,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-710439808"/>
+        <c:axId val="2077944576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-710436544"/>
+        <c:crossAx val="2077942944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1290,6 +1290,9 @@
                 <c:pt idx="2">
                   <c:v>92</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>89</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1305,11 +1308,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-710435456"/>
-        <c:axId val="-710432192"/>
+        <c:axId val="2077949472"/>
+        <c:axId val="2077950016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-710435456"/>
+        <c:axId val="2077949472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1413,7 +1416,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-710432192"/>
+        <c:crossAx val="2077950016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1421,7 +1424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-710432192"/>
+        <c:axId val="2077950016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1528,7 +1531,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-710435456"/>
+        <c:crossAx val="2077949472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3398,7 +3401,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3478,6 +3481,9 @@
         <f t="shared" si="0"/>
         <v>77.13</v>
       </c>
+      <c r="C6">
+        <v>89</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">

</xml_diff>

<commit_message>
Finished: Edit login details and account details
Signed on to do register new member
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -639,11 +639,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2077942944"/>
-        <c:axId val="2077944576"/>
+        <c:axId val="675071376"/>
+        <c:axId val="675073008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2077942944"/>
+        <c:axId val="675071376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -741,7 +741,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2077944576"/>
+        <c:crossAx val="675073008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -749,7 +749,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2077944576"/>
+        <c:axId val="675073008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2077942944"/>
+        <c:crossAx val="675071376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1293,6 +1293,9 @@
                 <c:pt idx="3">
                   <c:v>89</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>67</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1308,11 +1311,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2077949472"/>
-        <c:axId val="2077950016"/>
+        <c:axId val="1081955440"/>
+        <c:axId val="1081950000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2077949472"/>
+        <c:axId val="1081955440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1416,7 +1419,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2077950016"/>
+        <c:crossAx val="1081950000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1424,7 +1427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2077950016"/>
+        <c:axId val="1081950000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1531,7 +1534,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2077949472"/>
+        <c:crossAx val="1081955440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3401,7 +3404,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3493,6 +3496,10 @@
         <f t="shared" si="0"/>
         <v>72.84</v>
       </c>
+      <c r="C7">
+        <f>C6-22</f>
+        <v>67</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">

</xml_diff>

<commit_message>
FInished: register new member
Signed on to do event viewing event.
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -666,11 +666,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1085188672"/>
-        <c:axId val="-1085195200"/>
+        <c:axId val="2135404320"/>
+        <c:axId val="2129686768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1085188672"/>
+        <c:axId val="2135404320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -768,7 +768,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1085195200"/>
+        <c:crossAx val="2129686768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -776,7 +776,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1085195200"/>
+        <c:axId val="2129686768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,7 +882,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1085188672"/>
+        <c:crossAx val="2135404320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1323,6 +1323,9 @@
                 <c:pt idx="4">
                   <c:v>67</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>59</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1338,11 +1341,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1085188128"/>
-        <c:axId val="-1085193568"/>
+        <c:axId val="2129690576"/>
+        <c:axId val="2129694384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1085188128"/>
+        <c:axId val="2129690576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1446,7 +1449,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1085193568"/>
+        <c:crossAx val="2129694384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1454,7 +1457,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1085193568"/>
+        <c:axId val="2129694384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1561,7 +1564,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1085188128"/>
+        <c:crossAx val="2129690576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3431,7 +3434,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3574,6 +3577,10 @@
         <f t="shared" si="0"/>
         <v>68.55</v>
       </c>
+      <c r="C8">
+        <f>C7-8</f>
+        <v>59</v>
+      </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Finished attending events, almost events page
Events page needs to display the planners.
Also signed on to do volunteers list. That leaves 2 user stories for
each dan and ben
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -666,11 +666,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="937289728"/>
-        <c:axId val="937287552"/>
+        <c:axId val="-243175104"/>
+        <c:axId val="-243184352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="937289728"/>
+        <c:axId val="-243175104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -768,7 +768,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="937287552"/>
+        <c:crossAx val="-243184352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -776,7 +776,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="937287552"/>
+        <c:axId val="-243184352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,7 +882,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="937289728"/>
+        <c:crossAx val="-243175104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1332,6 +1332,33 @@
                 <c:pt idx="7">
                   <c:v>66</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1347,11 +1374,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="937288096"/>
-        <c:axId val="937290272"/>
+        <c:axId val="-243183808"/>
+        <c:axId val="-243180000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="937288096"/>
+        <c:axId val="-243183808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1378,11 +1405,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-AU"/>
-                  <a:t>Days Till release</a:t>
+                  <a:t>Days Till sprint</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-AU" baseline="0"/>
-                  <a:t> one</a:t>
+                  <a:t> release</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-AU"/>
               </a:p>
@@ -1455,7 +1482,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="937290272"/>
+        <c:crossAx val="-243180000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1463,7 +1490,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="937290272"/>
+        <c:axId val="-243180000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1570,7 +1597,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="937288096"/>
+        <c:crossAx val="-243183808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3439,8 +3466,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3639,6 +3666,9 @@
         <f t="shared" si="0"/>
         <v>55.68</v>
       </c>
+      <c r="C11">
+        <v>66</v>
+      </c>
       <c r="D11" t="s">
         <v>8</v>
       </c>
@@ -3654,6 +3684,9 @@
         <f t="shared" si="0"/>
         <v>51.39</v>
       </c>
+      <c r="C12">
+        <v>66</v>
+      </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
@@ -3669,6 +3702,9 @@
         <f t="shared" si="0"/>
         <v>47.1</v>
       </c>
+      <c r="C13">
+        <v>66</v>
+      </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
@@ -3684,6 +3720,9 @@
         <f t="shared" si="0"/>
         <v>42.81</v>
       </c>
+      <c r="C14">
+        <v>66</v>
+      </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
@@ -3699,6 +3738,9 @@
         <f t="shared" si="0"/>
         <v>38.520000000000003</v>
       </c>
+      <c r="C15">
+        <v>66</v>
+      </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
@@ -3714,6 +3756,9 @@
         <f t="shared" si="0"/>
         <v>34.229999999999997</v>
       </c>
+      <c r="C16">
+        <v>66</v>
+      </c>
       <c r="D16" t="s">
         <v>13</v>
       </c>
@@ -3729,6 +3774,9 @@
         <f t="shared" si="0"/>
         <v>29.94</v>
       </c>
+      <c r="C17">
+        <v>66</v>
+      </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
@@ -3744,6 +3792,9 @@
         <f t="shared" si="0"/>
         <v>25.65</v>
       </c>
+      <c r="C18">
+        <v>66</v>
+      </c>
       <c r="D18" t="s">
         <v>8</v>
       </c>
@@ -3758,6 +3809,10 @@
       <c r="B19">
         <f t="shared" si="0"/>
         <v>21.36</v>
+      </c>
+      <c r="C19">
+        <f>C18-16</f>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Finished volunteers list and view event
Were still alot behind guys. Please message me if you need help with
your tasks
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -666,11 +666,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-243175104"/>
-        <c:axId val="-243184352"/>
+        <c:axId val="210256704"/>
+        <c:axId val="210257248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-243175104"/>
+        <c:axId val="210256704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -768,7 +768,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-243184352"/>
+        <c:crossAx val="210257248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -776,7 +776,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-243184352"/>
+        <c:axId val="210257248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,7 +882,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-243175104"/>
+        <c:crossAx val="210256704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1359,6 +1359,12 @@
                 <c:pt idx="16">
                   <c:v>50</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1374,11 +1380,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-243183808"/>
-        <c:axId val="-243180000"/>
+        <c:axId val="430793744"/>
+        <c:axId val="430788848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-243183808"/>
+        <c:axId val="430793744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1482,7 +1488,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-243180000"/>
+        <c:crossAx val="430788848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1490,7 +1496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-243180000"/>
+        <c:axId val="430788848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1597,7 +1603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-243183808"/>
+        <c:crossAx val="430793744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3466,8 +3472,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3829,6 +3835,9 @@
         <f t="shared" si="0"/>
         <v>17.07</v>
       </c>
+      <c r="C20">
+        <v>50</v>
+      </c>
       <c r="D20" t="s">
         <v>10</v>
       </c>
@@ -3843,6 +3852,10 @@
       <c r="B21">
         <f t="shared" si="0"/>
         <v>12.78</v>
+      </c>
+      <c r="C21">
+        <f>C20-8</f>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Updated for todays tasks
Finished event registration, available events and edit event details
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -670,11 +670,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1643245424"/>
-        <c:axId val="-1643232912"/>
+        <c:axId val="-1952139152"/>
+        <c:axId val="-1952142960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1643245424"/>
+        <c:axId val="-1952139152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -772,7 +772,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1643232912"/>
+        <c:crossAx val="-1952142960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -780,7 +780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1643232912"/>
+        <c:axId val="-1952142960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,7 +886,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1643245424"/>
+        <c:crossAx val="-1952139152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1392,11 +1392,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1604951424"/>
-        <c:axId val="-1604950336"/>
+        <c:axId val="-1952145136"/>
+        <c:axId val="-1952151120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1604951424"/>
+        <c:axId val="-1952145136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1499,7 +1499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1604950336"/>
+        <c:crossAx val="-1952151120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1507,7 +1507,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1604950336"/>
+        <c:axId val="-1952151120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1613,7 +1613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1604951424"/>
+        <c:crossAx val="-1952145136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1999,6 +1999,9 @@
                 <c:pt idx="4">
                   <c:v>69</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>54</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2014,11 +2017,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1602673056"/>
-        <c:axId val="-1602666528"/>
+        <c:axId val="-1952146224"/>
+        <c:axId val="-1952142416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1602673056"/>
+        <c:axId val="-1952146224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2117,7 +2120,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1602666528"/>
+        <c:crossAx val="-1952142416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2125,7 +2128,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1602666528"/>
+        <c:axId val="-1952142416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2232,7 +2235,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1602673056"/>
+        <c:crossAx val="-1952146224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5141,7 +5144,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C7" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5305,6 +5308,10 @@
         <f t="shared" si="0"/>
         <v>61.714285714285701</v>
       </c>
+      <c r="C8">
+        <f>C7-F8</f>
+        <v>54</v>
+      </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
@@ -5312,7 +5319,7 @@
         <v>42658</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
miscounted how many tasks we had. Everthing adds up now
also updated it
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -670,11 +670,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1952139152"/>
-        <c:axId val="-1952142960"/>
+        <c:axId val="1437938560"/>
+        <c:axId val="1437934208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1952139152"/>
+        <c:axId val="1437938560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -772,7 +772,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1952142960"/>
+        <c:crossAx val="1437934208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -780,7 +780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1952142960"/>
+        <c:axId val="1437934208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,7 +886,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1952139152"/>
+        <c:crossAx val="1437938560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1392,11 +1392,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1952145136"/>
-        <c:axId val="-1952151120"/>
+        <c:axId val="1438401872"/>
+        <c:axId val="1438408944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1952145136"/>
+        <c:axId val="1438401872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1499,7 +1499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1952151120"/>
+        <c:crossAx val="1438408944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1507,7 +1507,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1952151120"/>
+        <c:axId val="1438408944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1613,7 +1613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1952145136"/>
+        <c:crossAx val="1438401872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1837,49 +1837,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>96</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89.142857142857139</c:v>
+                  <c:v>93.785714285714292</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>82.285714285714278</c:v>
+                  <c:v>86.571428571428584</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.428571428571416</c:v>
+                  <c:v>79.357142857142875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68.571428571428555</c:v>
+                  <c:v>72.142857142857167</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>61.714285714285701</c:v>
+                  <c:v>64.928571428571459</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>54.857142857142847</c:v>
+                  <c:v>57.714285714285744</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>47.999999999999993</c:v>
+                  <c:v>50.500000000000028</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41.142857142857139</c:v>
+                  <c:v>43.285714285714313</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.285714285714285</c:v>
+                  <c:v>36.071428571428598</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.428571428571427</c:v>
+                  <c:v>28.857142857142883</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.571428571428569</c:v>
+                  <c:v>21.642857142857167</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.714285714285712</c:v>
+                  <c:v>14.428571428571452</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.857142857142855</c:v>
+                  <c:v>7.2142857142857375</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>2.3092638912203256E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1985,22 +1985,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>96</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>85</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>85</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>69</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54</c:v>
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2017,11 +2020,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1952146224"/>
-        <c:axId val="-1952142416"/>
+        <c:axId val="1436951392"/>
+        <c:axId val="1791677312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1952146224"/>
+        <c:axId val="1436951392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2120,7 +2123,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1952142416"/>
+        <c:crossAx val="1791677312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2128,7 +2131,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1952142416"/>
+        <c:axId val="1791677312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2235,7 +2238,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1952146224"/>
+        <c:crossAx val="1436951392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5144,7 +5147,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C8"/>
+      <selection activeCell="C8" sqref="C8:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5191,10 +5194,10 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C3">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -5218,11 +5221,11 @@
       </c>
       <c r="B4">
         <f xml:space="preserve"> B3 - ($B$3/14)</f>
-        <v>89.142857142857139</v>
+        <v>93.785714285714292</v>
       </c>
       <c r="C4">
         <f>C3-F4</f>
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -5240,11 +5243,11 @@
       </c>
       <c r="B5">
         <f xml:space="preserve"> B4 - ($B$3/14)</f>
-        <v>82.285714285714278</v>
+        <v>86.571428571428584</v>
       </c>
       <c r="C5">
         <f>C4-F5</f>
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -5262,11 +5265,11 @@
       </c>
       <c r="B6">
         <f t="shared" ref="B6:B17" si="0" xml:space="preserve"> B5 - ($B$3/14)</f>
-        <v>75.428571428571416</v>
+        <v>79.357142857142875</v>
       </c>
       <c r="C6">
         <f>C5-F6</f>
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -5284,11 +5287,11 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>68.571428571428555</v>
+        <v>72.142857142857167</v>
       </c>
       <c r="C7">
         <f>C6-F7</f>
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -5306,11 +5309,11 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>61.714285714285701</v>
+        <v>64.928571428571459</v>
       </c>
       <c r="C8">
         <f>C7-F8</f>
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -5328,7 +5331,11 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>54.857142857142847</v>
+        <v>57.714285714285744</v>
+      </c>
+      <c r="C9">
+        <f>C8-F9</f>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -5346,7 +5353,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>47.999999999999993</v>
+        <v>50.500000000000028</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -5364,7 +5371,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>41.142857142857139</v>
+        <v>43.285714285714313</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -5382,7 +5389,7 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>34.285714285714285</v>
+        <v>36.071428571428598</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -5400,7 +5407,7 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>27.428571428571427</v>
+        <v>28.857142857142883</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -5418,7 +5425,7 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>20.571428571428569</v>
+        <v>21.642857142857167</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -5436,7 +5443,7 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>13.714285714285712</v>
+        <v>14.428571428571452</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -5454,7 +5461,7 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>6.857142857142855</v>
+        <v>7.2142857142857375</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -5472,7 +5479,7 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.3092638912203256E-14</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Helped lance finished the register new volunteer
I made the Add_new_volunteer.php.
While lance the made the Volunteer_account_details.php
</commit_message>
<xml_diff>
--- a/Burndown chart.xlsx
+++ b/Burndown chart.xlsx
@@ -670,11 +670,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1437938560"/>
-        <c:axId val="1437934208"/>
+        <c:axId val="844088496"/>
+        <c:axId val="844091216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1437938560"/>
+        <c:axId val="844088496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -772,7 +772,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1437934208"/>
+        <c:crossAx val="844091216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -780,7 +780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1437934208"/>
+        <c:axId val="844091216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,7 +886,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1437938560"/>
+        <c:crossAx val="844088496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1392,11 +1392,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1438401872"/>
-        <c:axId val="1438408944"/>
+        <c:axId val="706228208"/>
+        <c:axId val="706216784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1438401872"/>
+        <c:axId val="706228208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1499,7 +1499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1438408944"/>
+        <c:crossAx val="706216784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1507,7 +1507,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1438408944"/>
+        <c:axId val="706216784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1613,7 +1613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1438401872"/>
+        <c:crossAx val="706228208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1837,49 +1837,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>101</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>93.785714285714292</c:v>
+                  <c:v>87.285714285714292</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86.571428571428584</c:v>
+                  <c:v>80.571428571428584</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>79.357142857142875</c:v>
+                  <c:v>73.857142857142875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>72.142857142857167</c:v>
+                  <c:v>67.142857142857167</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>64.928571428571459</c:v>
+                  <c:v>60.428571428571452</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.714285714285744</c:v>
+                  <c:v>53.714285714285737</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50.500000000000028</c:v>
+                  <c:v>47.000000000000021</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43.285714285714313</c:v>
+                  <c:v>40.285714285714306</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36.071428571428598</c:v>
+                  <c:v>33.571428571428591</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28.857142857142883</c:v>
+                  <c:v>26.857142857142875</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21.642857142857167</c:v>
+                  <c:v>20.14285714285716</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14.428571428571452</c:v>
+                  <c:v>13.428571428571445</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.2142857142857375</c:v>
+                  <c:v>6.7142857142857304</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3092638912203256E-14</c:v>
+                  <c:v>1.5987211554602254E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1985,25 +1985,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>101</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>95</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>74</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>59</c:v>
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2020,11 +2023,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1436951392"/>
-        <c:axId val="1791677312"/>
+        <c:axId val="675377424"/>
+        <c:axId val="675374704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1436951392"/>
+        <c:axId val="675377424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2123,7 +2126,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1791677312"/>
+        <c:crossAx val="675374704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2131,7 +2134,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1791677312"/>
+        <c:axId val="675374704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2238,7 +2241,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1436951392"/>
+        <c:crossAx val="675377424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5147,7 +5150,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5194,10 +5197,10 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C3">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -5221,11 +5224,11 @@
       </c>
       <c r="B4">
         <f xml:space="preserve"> B3 - ($B$3/14)</f>
-        <v>93.785714285714292</v>
+        <v>87.285714285714292</v>
       </c>
       <c r="C4">
-        <f>C3-F4</f>
-        <v>95</v>
+        <f t="shared" ref="C4:C10" si="0">C3-F4</f>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -5243,11 +5246,11 @@
       </c>
       <c r="B5">
         <f xml:space="preserve"> B4 - ($B$3/14)</f>
-        <v>86.571428571428584</v>
+        <v>80.571428571428584</v>
       </c>
       <c r="C5">
-        <f>C4-F5</f>
-        <v>90</v>
+        <f t="shared" si="0"/>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -5264,12 +5267,12 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:B17" si="0" xml:space="preserve"> B5 - ($B$3/14)</f>
-        <v>79.357142857142875</v>
+        <f t="shared" ref="B6:B17" si="1" xml:space="preserve"> B5 - ($B$3/14)</f>
+        <v>73.857142857142875</v>
       </c>
       <c r="C6">
-        <f>C5-F6</f>
-        <v>90</v>
+        <f t="shared" si="0"/>
+        <v>83</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -5286,12 +5289,12 @@
         <v>10</v>
       </c>
       <c r="B7">
+        <f t="shared" si="1"/>
+        <v>67.142857142857167</v>
+      </c>
+      <c r="C7">
         <f t="shared" si="0"/>
-        <v>72.142857142857167</v>
-      </c>
-      <c r="C7">
-        <f>C6-F7</f>
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -5308,12 +5311,12 @@
         <v>9</v>
       </c>
       <c r="B8">
+        <f t="shared" si="1"/>
+        <v>60.428571428571452</v>
+      </c>
+      <c r="C8">
         <f t="shared" si="0"/>
-        <v>64.928571428571459</v>
-      </c>
-      <c r="C8">
-        <f>C7-F8</f>
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -5330,12 +5333,12 @@
         <v>8</v>
       </c>
       <c r="B9">
+        <f t="shared" si="1"/>
+        <v>53.714285714285737</v>
+      </c>
+      <c r="C9">
         <f t="shared" si="0"/>
-        <v>57.714285714285744</v>
-      </c>
-      <c r="C9">
-        <f>C8-F9</f>
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -5352,8 +5355,12 @@
         <v>7</v>
       </c>
       <c r="B10">
+        <f t="shared" si="1"/>
+        <v>47.000000000000021</v>
+      </c>
+      <c r="C10">
         <f t="shared" si="0"/>
-        <v>50.500000000000028</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -5362,7 +5369,7 @@
         <v>42660</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5370,8 +5377,8 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
-        <v>43.285714285714313</v>
+        <f t="shared" si="1"/>
+        <v>40.285714285714306</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -5388,8 +5395,8 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
-        <v>36.071428571428598</v>
+        <f t="shared" si="1"/>
+        <v>33.571428571428591</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -5406,8 +5413,8 @@
         <v>4</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
-        <v>28.857142857142883</v>
+        <f t="shared" si="1"/>
+        <v>26.857142857142875</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -5424,8 +5431,8 @@
         <v>3</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
-        <v>21.642857142857167</v>
+        <f t="shared" si="1"/>
+        <v>20.14285714285716</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -5442,8 +5449,8 @@
         <v>2</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
-        <v>14.428571428571452</v>
+        <f t="shared" si="1"/>
+        <v>13.428571428571445</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -5460,8 +5467,8 @@
         <v>1</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
-        <v>7.2142857142857375</v>
+        <f t="shared" si="1"/>
+        <v>6.7142857142857304</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -5478,8 +5485,8 @@
         <v>0</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
-        <v>2.3092638912203256E-14</v>
+        <f t="shared" si="1"/>
+        <v>1.5987211554602254E-14</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>

</xml_diff>